<commit_message>
Scrum Board & Phase1.Sprint1.SprintBacklog updated
Signed-off-by: GoncaloRodri <gg.rodrigues@campus.fct.unl.pt>
</commit_message>
<xml_diff>
--- a/project/Phase1/Sprint1/Sprint Backlog.xlsx
+++ b/project/Phase1/Sprint1/Sprint Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Backlog</t>
   </si>
@@ -31,37 +31,82 @@
     <t>Identify Code Smells</t>
   </si>
   <si>
-    <t>Identify 3 Code Smells in "Option" Folder - Gonçalo Rodrigues</t>
+    <t>Identify 3 Code Smells 
+By: Gonçalo Rodrigues</t>
   </si>
   <si>
-    <t>Identify 3 Code Smells in "Time" Folder - Gonçalo Gomes</t>
+    <t>-&gt;</t>
   </si>
   <si>
-    <t>Identify 3 Code Smells in "Calendar" Folder - Guilherme Santana</t>
+    <t>Identify 3 Code Smells 
+By: Gonçalo Rodrigues 
+Reviewers:Joana Cruz, Bárbara Correia. Guilherme Santana</t>
   </si>
   <si>
-    <t>Identify 3 Code Smells in "io" &amp; "Task" Folders - Bárbara Correia</t>
+    <t>Identify 3 Code Smells 
+By: Gonçalo Gomes</t>
   </si>
   <si>
-    <t>Identify 3 Code Smells in other Folders - Joana Cruz</t>
+    <t>Identify 3 Code Smells
+By: Guilherme Santana</t>
+  </si>
+  <si>
+    <t>Identify 3 Code Smells 
+By: Guilherme Santana</t>
+  </si>
+  <si>
+    <t>Identify 3 Code Smells 
+By: Bárbara Correia</t>
+  </si>
+  <si>
+    <t>Identify 3 Code Smells
+By: Bárbara Correia</t>
+  </si>
+  <si>
+    <t>Identify 3 Code Smells 
+By: Joana Cruz</t>
+  </si>
+  <si>
+    <t>Identify 3 Code Smells i
+By: Joana Cruz</t>
+  </si>
+  <si>
+    <t>Identify 3 Code Smells 
+By:  Joana Cruz 
+Reviewers: Bárbara Correia, Gonçalo Rodrigues, Gonçalo Gomes</t>
   </si>
   <si>
     <t>Identify Design Patterns</t>
   </si>
   <si>
-    <t>Identify 3 Pattern Designs in "Option" Folder - Gonçalo Rodrigues</t>
+    <t>Identify 3 Pattern Designs 
+By: Gonçalo Rodrigues</t>
   </si>
   <si>
-    <t>Identify 3 Pattern Designs in "Time" Folder - Gonçalo Gomes</t>
+    <t>Identify 3 Pattern Designs 
+By: Gonçalo Rodrigues 
+Reviewers:Joana Cruz, Bárbara Correia. Guilherme Santana</t>
   </si>
   <si>
-    <t>Identify 3 Pattern Designs in "Calendar" Folder - Guilherme Santana</t>
+    <t>Identify 3 Pattern Designs 
+By: Gonçalo Gomes</t>
   </si>
   <si>
-    <t>Identify 3 Pattern Designs in "io" &amp; "Task" Folders - Bárbara Correia</t>
+    <t>Identify 3 Pattern Designs
+By: Guilherme Santana</t>
   </si>
   <si>
-    <t>Identify 3 Pattern Designs in other Folders - Joana Cruz</t>
+    <t>Identify 3 Pattern Designs 
+By: Bárbara Correia</t>
+  </si>
+  <si>
+    <t>Identify 3 Pattern Designs 
+By: Joana Cruz</t>
+  </si>
+  <si>
+    <t>Identify 3 Pattern Designs 
+By: Joana Cruz 
+Reviewers: Bárbara Correia, Gonçalo Rodrigues, Gonçalo Gomes</t>
   </si>
 </sst>
 </file>
@@ -154,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -175,8 +220,14 @@
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -195,9 +246,6 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -433,19 +481,6 @@
     <col customWidth="1" min="23" max="29" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
     <row r="3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -495,7 +530,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" ht="55.5" customHeight="1">
+    <row r="6" ht="89.25" customHeight="1">
       <c r="B6" s="1"/>
       <c r="C6" s="6" t="s">
         <v>5</v>
@@ -504,134 +539,210 @@
       <c r="E6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="F6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" ht="89.25" customHeight="1">
       <c r="B7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="G7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8">
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="10" t="s">
-        <v>8</v>
+      <c r="E8" s="12" t="s">
+        <v>10</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="F8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="11" t="s">
-        <v>9</v>
+      <c r="E9" s="13" t="s">
+        <v>12</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="F9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="10"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="B10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="12" t="s">
-        <v>10</v>
+      <c r="E10" s="14" t="s">
+        <v>14</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="F10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="10"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="B11" s="1"/>
-      <c r="C11" s="13"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="B12" s="1"/>
       <c r="C12" s="6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="F12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="9" t="s">
-        <v>13</v>
+      <c r="E13" s="11" t="s">
+        <v>20</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="F13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="10"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="10" t="s">
-        <v>14</v>
+      <c r="E14" s="12" t="s">
+        <v>21</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="F14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="10"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="11" t="s">
-        <v>15</v>
+      <c r="E15" s="13" t="s">
+        <v>22</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="F15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="12" t="s">
-        <v>16</v>
+      <c r="E16" s="14" t="s">
+        <v>23</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="F16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -639,12 +750,12 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -670,7 +781,7 @@
       <c r="H20" s="1"/>
       <c r="J20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="V20" s="16"/>
+      <c r="V20" s="17"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="B21" s="1"/>

</xml_diff>